<commit_message>
First commit inject 70-275
</commit_message>
<xml_diff>
--- a/examples/EUMFH/summary_AR-gc.xlsx
+++ b/examples/EUMFH/summary_AR-gc.xlsx
@@ -19,8 +19,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Giorgio Cangioli</author>
+  </authors>
+  <commentList>
+    <comment ref="O4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Giorgio Cangioli:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is a procedure</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="157">
   <si>
     <t>Inject</t>
   </si>
@@ -486,13 +520,19 @@
   </si>
   <si>
     <t>Birthdate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZMAJE </t>
+  </si>
+  <si>
+    <t>vaccine dates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,8 +556,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,6 +598,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -576,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -606,6 +665,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -929,11 +995,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,37 +1026,37 @@
     <col min="22" max="22" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:29" s="9" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="C1" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="18" t="s">
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19" t="s">
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-    </row>
-    <row r="2" spans="1:26" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+    </row>
+    <row r="2" spans="1:29" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -1067,7 +1133,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>51</v>
       </c>
@@ -1110,8 +1176,12 @@
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
-    </row>
-    <row r="4" spans="1:26" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z3">
+        <f>2018-E3</f>
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>52</v>
       </c>
@@ -1181,11 +1251,11 @@
         <v>7</v>
       </c>
       <c r="Z4">
-        <f>2018-61</f>
+        <f t="shared" ref="Z4:Z15" si="0">2018-E4</f>
         <v>1957</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>61</v>
       </c>
@@ -1228,8 +1298,12 @@
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
-    </row>
-    <row r="6" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Z5">
+        <f t="shared" si="0"/>
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>62</v>
       </c>
@@ -1276,8 +1350,12 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
-    </row>
-    <row r="7" spans="1:26" ht="28.9" x14ac:dyDescent="0.3">
+      <c r="Z6">
+        <f t="shared" si="0"/>
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>63</v>
       </c>
@@ -1324,8 +1402,12 @@
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Z7">
+        <f t="shared" si="0"/>
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>92</v>
       </c>
@@ -1368,8 +1450,12 @@
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
-    </row>
-    <row r="9" spans="1:26" ht="115.15" x14ac:dyDescent="0.3">
+      <c r="Z8">
+        <f t="shared" si="0"/>
+        <v>1946</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="115.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>44</v>
       </c>
@@ -1403,10 +1489,10 @@
       <c r="K9" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="L9" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M9" s="20" t="s">
         <v>145</v>
       </c>
       <c r="N9" s="3" t="s">
@@ -1415,7 +1501,7 @@
       <c r="O9" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="P9" s="3" t="s">
+      <c r="P9" s="18" t="s">
         <v>141</v>
       </c>
       <c r="Q9" s="3" t="s">
@@ -1430,8 +1516,21 @@
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
-    </row>
-    <row r="10" spans="1:26" ht="115.15" x14ac:dyDescent="0.3">
+      <c r="X9" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y9">
+        <v>275</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="0"/>
+        <v>1988</v>
+      </c>
+      <c r="AC9" s="19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>100</v>
       </c>
@@ -1474,8 +1573,12 @@
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
-    </row>
-    <row r="11" spans="1:26" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="Z10">
+        <f t="shared" si="0"/>
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>23</v>
       </c>
@@ -1518,8 +1621,12 @@
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
-    </row>
-    <row r="12" spans="1:26" ht="43.15" x14ac:dyDescent="0.3">
+      <c r="Z11">
+        <f t="shared" si="0"/>
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>105</v>
       </c>
@@ -1560,8 +1667,12 @@
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
-    </row>
-    <row r="13" spans="1:26" ht="43.15" x14ac:dyDescent="0.3">
+      <c r="Z12">
+        <f t="shared" si="0"/>
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>36</v>
       </c>
@@ -1606,8 +1717,12 @@
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
-    </row>
-    <row r="14" spans="1:26" ht="28.9" x14ac:dyDescent="0.3">
+      <c r="Z13">
+        <f t="shared" si="0"/>
+        <v>1963</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>42</v>
       </c>
@@ -1652,8 +1767,12 @@
         <v>148</v>
       </c>
       <c r="V14" s="4"/>
-    </row>
-    <row r="15" spans="1:26" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z14">
+        <f t="shared" si="0"/>
+        <v>1969</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>64</v>
       </c>
@@ -1700,8 +1819,12 @@
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
-    </row>
-    <row r="16" spans="1:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z15">
+        <f t="shared" si="0"/>
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
@@ -1733,6 +1856,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>